<commit_message>
add pearson to text_similarity.ipynb
</commit_message>
<xml_diff>
--- a/data/Paired Image.xlsx
+++ b/data/Paired Image.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/880d6679c26b7b92/Desktop/SC4020-Project-1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_6441F3A5D3805D6EAB9B2C11595ED87656CD3F48" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{535FB8DD-FA2B-4F4A-AC4B-A6C336ED3E74}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_6441F3A5D3805D6EAB9B2C11595ED87656CD3F48" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD96FA71-32E5-4CAB-B1D1-FAF7FA9EB827}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="304">
   <si>
     <t>Image 1</t>
   </si>
@@ -929,6 +929,9 @@
   </si>
   <si>
     <t>2877159456_ea4a46b0d2.jpg</t>
+  </si>
+  <si>
+    <t>146577645_91b570c0d0.jpg</t>
   </si>
 </sst>
 </file>
@@ -993,7 +996,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1004,6 +1015,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1291,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F153" sqref="F153"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2964,7 +2979,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>303</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>